<commit_message>
Add plotting extensions section to ch4
</commit_message>
<xml_diff>
--- a/data/sample_qog_bas_ts_jan23.xlsx
+++ b/data/sample_qog_bas_ts_jan23.xlsx
@@ -4246,7 +4246,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -4280,7 +4280,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -4314,7 +4314,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4348,7 +4348,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4382,7 +4382,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4484,7 +4484,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4518,7 +4518,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4586,7 +4586,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4620,7 +4620,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4654,7 +4654,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4688,7 +4688,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4722,7 +4722,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4756,7 +4756,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -4790,7 +4790,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4824,7 +4824,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4858,7 +4858,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4892,7 +4892,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4926,7 +4926,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4960,7 +4960,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4994,7 +4994,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -5028,7 +5028,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -5062,7 +5062,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -5096,7 +5096,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -5130,7 +5130,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -5164,7 +5164,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -5198,7 +5198,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -5232,7 +5232,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -5266,7 +5266,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -32642,7 +32642,7 @@
     <row r="994">
       <c r="A994" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B994" t="inlineStr">
@@ -32676,7 +32676,7 @@
     <row r="995">
       <c r="A995" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B995" t="inlineStr">
@@ -32710,7 +32710,7 @@
     <row r="996">
       <c r="A996" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B996" t="inlineStr">
@@ -32744,7 +32744,7 @@
     <row r="997">
       <c r="A997" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B997" t="inlineStr">
@@ -32778,7 +32778,7 @@
     <row r="998">
       <c r="A998" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B998" t="inlineStr">
@@ -32812,7 +32812,7 @@
     <row r="999">
       <c r="A999" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B999" t="inlineStr">
@@ -32846,7 +32846,7 @@
     <row r="1000">
       <c r="A1000" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1000" t="inlineStr">
@@ -32880,7 +32880,7 @@
     <row r="1001">
       <c r="A1001" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1001" t="inlineStr">
@@ -32914,7 +32914,7 @@
     <row r="1002">
       <c r="A1002" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1002" t="inlineStr">
@@ -32948,7 +32948,7 @@
     <row r="1003">
       <c r="A1003" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1003" t="inlineStr">
@@ -32982,7 +32982,7 @@
     <row r="1004">
       <c r="A1004" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1004" t="inlineStr">
@@ -33016,7 +33016,7 @@
     <row r="1005">
       <c r="A1005" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1005" t="inlineStr">
@@ -33050,7 +33050,7 @@
     <row r="1006">
       <c r="A1006" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1006" t="inlineStr">
@@ -33084,7 +33084,7 @@
     <row r="1007">
       <c r="A1007" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1007" t="inlineStr">
@@ -33118,7 +33118,7 @@
     <row r="1008">
       <c r="A1008" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1008" t="inlineStr">
@@ -33152,7 +33152,7 @@
     <row r="1009">
       <c r="A1009" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1009" t="inlineStr">
@@ -33186,7 +33186,7 @@
     <row r="1010">
       <c r="A1010" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1010" t="inlineStr">
@@ -33220,7 +33220,7 @@
     <row r="1011">
       <c r="A1011" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1011" t="inlineStr">
@@ -33254,7 +33254,7 @@
     <row r="1012">
       <c r="A1012" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1012" t="inlineStr">
@@ -33288,7 +33288,7 @@
     <row r="1013">
       <c r="A1013" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1013" t="inlineStr">
@@ -33322,7 +33322,7 @@
     <row r="1014">
       <c r="A1014" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1014" t="inlineStr">
@@ -33356,7 +33356,7 @@
     <row r="1015">
       <c r="A1015" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1015" t="inlineStr">
@@ -33390,7 +33390,7 @@
     <row r="1016">
       <c r="A1016" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1016" t="inlineStr">
@@ -33424,7 +33424,7 @@
     <row r="1017">
       <c r="A1017" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1017" t="inlineStr">
@@ -33458,7 +33458,7 @@
     <row r="1018">
       <c r="A1018" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1018" t="inlineStr">
@@ -33492,7 +33492,7 @@
     <row r="1019">
       <c r="A1019" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1019" t="inlineStr">
@@ -33526,7 +33526,7 @@
     <row r="1020">
       <c r="A1020" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1020" t="inlineStr">
@@ -33560,7 +33560,7 @@
     <row r="1021">
       <c r="A1021" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1021" t="inlineStr">
@@ -33594,7 +33594,7 @@
     <row r="1022">
       <c r="A1022" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1022" t="inlineStr">
@@ -33628,7 +33628,7 @@
     <row r="1023">
       <c r="A1023" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1023" t="inlineStr">
@@ -33662,7 +33662,7 @@
     <row r="1024">
       <c r="A1024" t="inlineStr">
         <is>
-          <t>United States of America (the)</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B1024" t="inlineStr">
@@ -34750,7 +34750,7 @@
     <row r="1056">
       <c r="A1056" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1056" t="inlineStr">
@@ -34784,7 +34784,7 @@
     <row r="1057">
       <c r="A1057" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1057" t="inlineStr">
@@ -34818,7 +34818,7 @@
     <row r="1058">
       <c r="A1058" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1058" t="inlineStr">
@@ -34852,7 +34852,7 @@
     <row r="1059">
       <c r="A1059" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1059" t="inlineStr">
@@ -34886,7 +34886,7 @@
     <row r="1060">
       <c r="A1060" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1060" t="inlineStr">
@@ -34920,7 +34920,7 @@
     <row r="1061">
       <c r="A1061" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1061" t="inlineStr">
@@ -34954,7 +34954,7 @@
     <row r="1062">
       <c r="A1062" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1062" t="inlineStr">
@@ -34988,7 +34988,7 @@
     <row r="1063">
       <c r="A1063" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1063" t="inlineStr">
@@ -35022,7 +35022,7 @@
     <row r="1064">
       <c r="A1064" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1064" t="inlineStr">
@@ -35056,7 +35056,7 @@
     <row r="1065">
       <c r="A1065" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1065" t="inlineStr">
@@ -35090,7 +35090,7 @@
     <row r="1066">
       <c r="A1066" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1066" t="inlineStr">
@@ -35124,7 +35124,7 @@
     <row r="1067">
       <c r="A1067" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1067" t="inlineStr">
@@ -35158,7 +35158,7 @@
     <row r="1068">
       <c r="A1068" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1068" t="inlineStr">
@@ -35192,7 +35192,7 @@
     <row r="1069">
       <c r="A1069" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1069" t="inlineStr">
@@ -35226,7 +35226,7 @@
     <row r="1070">
       <c r="A1070" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1070" t="inlineStr">
@@ -35260,7 +35260,7 @@
     <row r="1071">
       <c r="A1071" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1071" t="inlineStr">
@@ -35294,7 +35294,7 @@
     <row r="1072">
       <c r="A1072" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1072" t="inlineStr">
@@ -35328,7 +35328,7 @@
     <row r="1073">
       <c r="A1073" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1073" t="inlineStr">
@@ -35362,7 +35362,7 @@
     <row r="1074">
       <c r="A1074" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1074" t="inlineStr">
@@ -35396,7 +35396,7 @@
     <row r="1075">
       <c r="A1075" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1075" t="inlineStr">
@@ -35430,7 +35430,7 @@
     <row r="1076">
       <c r="A1076" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1076" t="inlineStr">
@@ -35464,7 +35464,7 @@
     <row r="1077">
       <c r="A1077" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1077" t="inlineStr">
@@ -35498,7 +35498,7 @@
     <row r="1078">
       <c r="A1078" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1078" t="inlineStr">
@@ -35532,7 +35532,7 @@
     <row r="1079">
       <c r="A1079" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1079" t="inlineStr">
@@ -35566,7 +35566,7 @@
     <row r="1080">
       <c r="A1080" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1080" t="inlineStr">
@@ -35600,7 +35600,7 @@
     <row r="1081">
       <c r="A1081" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1081" t="inlineStr">
@@ -35634,7 +35634,7 @@
     <row r="1082">
       <c r="A1082" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1082" t="inlineStr">
@@ -35668,7 +35668,7 @@
     <row r="1083">
       <c r="A1083" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1083" t="inlineStr">
@@ -35702,7 +35702,7 @@
     <row r="1084">
       <c r="A1084" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1084" t="inlineStr">
@@ -35736,7 +35736,7 @@
     <row r="1085">
       <c r="A1085" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1085" t="inlineStr">
@@ -35770,7 +35770,7 @@
     <row r="1086">
       <c r="A1086" t="inlineStr">
         <is>
-          <t>Venezuela (Bolivarian Republic of)</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B1086" t="inlineStr">

</xml_diff>